<commit_message>
component_classes ready, next working on building_classes
</commit_message>
<xml_diff>
--- a/Satisfactory_calculator/item_list.xlsx
+++ b/Satisfactory_calculator/item_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjarki\source\repos\Satisfactory_calculator\Satisfactory_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CBB592-CCDA-4898-9E0E-333AACA4FCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4CFEAD-CA80-44D9-9E70-BA1B3C25050C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21000" activeTab="1" xr2:uid="{CF63DFE2-E3F1-40A6-9DC4-F78A2094206C}"/>
+    <workbookView xWindow="5340" yWindow="2760" windowWidth="30405" windowHeight="14295" activeTab="3" xr2:uid="{CF63DFE2-E3F1-40A6-9DC4-F78A2094206C}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_material" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8234" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8234" uniqueCount="1348">
   <si>
     <t>Crafted In</t>
   </si>
@@ -4071,6 +4071,12 @@
   </si>
   <si>
     <t>Dissolved Silica</t>
+  </si>
+  <si>
+    <t>item_qty_1</t>
+  </si>
+  <si>
+    <t>item_qty_unit_1</t>
   </si>
 </sst>
 </file>
@@ -4134,10 +4140,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7286,33 +7292,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C4349C-A20E-4466-BDDA-F12F53635295}">
   <dimension ref="A1:V316"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A244" sqref="A244:XFD244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7324,10 +7330,10 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>1346</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>1347</v>
       </c>
       <c r="E1" t="s">
         <v>1328</v>
@@ -7409,7 +7415,7 @@
       <c r="J2" t="s">
         <v>1337</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>5</v>
       </c>
       <c r="L2" t="s">
@@ -21772,7 +21778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F544B06-6065-4C8E-AAF6-1E1D3DDA6940}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B57" sqref="B56:B57"/>
     </sheetView>
   </sheetViews>
@@ -22032,8 +22038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA56A5F-A7B5-4952-A980-96BA279343B3}">
   <dimension ref="A1:AK922"/>
   <sheetViews>
-    <sheetView topLeftCell="A608" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A656" sqref="A656:XFD656"/>
+    <sheetView topLeftCell="N472" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C497" sqref="C497:X497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27470,7 +27476,7 @@
       <c r="AH143" s="1"/>
       <c r="AI143" s="1"/>
       <c r="AJ143" s="2"/>
-      <c r="AK143" s="4"/>
+      <c r="AK143" s="5"/>
     </row>
     <row r="144" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
@@ -27526,7 +27532,7 @@
       <c r="AH144" s="1"/>
       <c r="AI144" s="1"/>
       <c r="AJ144" s="3"/>
-      <c r="AK144" s="4"/>
+      <c r="AK144" s="5"/>
     </row>
     <row r="145" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
@@ -27588,7 +27594,7 @@
       <c r="AH145" s="1"/>
       <c r="AI145" s="1"/>
       <c r="AJ145" s="1"/>
-      <c r="AK145" s="4"/>
+      <c r="AK145" s="5"/>
     </row>
     <row r="146" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
@@ -27842,7 +27848,7 @@
       <c r="AH149" s="1"/>
       <c r="AI149" s="1"/>
       <c r="AJ149" s="2"/>
-      <c r="AK149" s="4"/>
+      <c r="AK149" s="5"/>
     </row>
     <row r="150" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
@@ -27910,7 +27916,7 @@
       <c r="AH150" s="1"/>
       <c r="AI150" s="1"/>
       <c r="AJ150" s="3"/>
-      <c r="AK150" s="4"/>
+      <c r="AK150" s="5"/>
     </row>
     <row r="151" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
@@ -27972,7 +27978,7 @@
       <c r="AH151" s="1"/>
       <c r="AI151" s="1"/>
       <c r="AJ151" s="1"/>
-      <c r="AK151" s="4"/>
+      <c r="AK151" s="5"/>
     </row>
     <row r="152" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
@@ -28096,7 +28102,7 @@
       <c r="AH153" s="1"/>
       <c r="AI153" s="1"/>
       <c r="AJ153" s="2"/>
-      <c r="AK153" s="4"/>
+      <c r="AK153" s="5"/>
     </row>
     <row r="154" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
@@ -28176,7 +28182,7 @@
       <c r="AH154" s="1"/>
       <c r="AI154" s="1"/>
       <c r="AJ154" s="3"/>
-      <c r="AK154" s="4"/>
+      <c r="AK154" s="5"/>
     </row>
     <row r="155" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
@@ -28232,7 +28238,7 @@
       <c r="AH155" s="1"/>
       <c r="AI155" s="1"/>
       <c r="AJ155" s="1"/>
-      <c r="AK155" s="4"/>
+      <c r="AK155" s="5"/>
     </row>
     <row r="156" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
@@ -28424,7 +28430,7 @@
       <c r="AH158" s="1"/>
       <c r="AI158" s="1"/>
       <c r="AJ158" s="2"/>
-      <c r="AK158" s="4"/>
+      <c r="AK158" s="5"/>
     </row>
     <row r="159" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
@@ -28480,7 +28486,7 @@
       <c r="AH159" s="1"/>
       <c r="AI159" s="1"/>
       <c r="AJ159" s="3"/>
-      <c r="AK159" s="4"/>
+      <c r="AK159" s="5"/>
     </row>
     <row r="160" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
@@ -28542,7 +28548,7 @@
       <c r="AH160" s="1"/>
       <c r="AI160" s="1"/>
       <c r="AJ160" s="1"/>
-      <c r="AK160" s="4"/>
+      <c r="AK160" s="5"/>
     </row>
     <row r="161" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
@@ -28610,7 +28616,7 @@
       <c r="AH161" s="1"/>
       <c r="AI161" s="1"/>
       <c r="AJ161" s="2"/>
-      <c r="AK161" s="4"/>
+      <c r="AK161" s="5"/>
     </row>
     <row r="162" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
@@ -28672,7 +28678,7 @@
       <c r="AH162" s="1"/>
       <c r="AI162" s="1"/>
       <c r="AJ162" s="3"/>
-      <c r="AK162" s="4"/>
+      <c r="AK162" s="5"/>
     </row>
     <row r="163" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
@@ -28734,7 +28740,7 @@
       <c r="AH163" s="1"/>
       <c r="AI163" s="1"/>
       <c r="AJ163" s="1"/>
-      <c r="AK163" s="4"/>
+      <c r="AK163" s="5"/>
     </row>
     <row r="164" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
@@ -28802,7 +28808,7 @@
       <c r="AH164" s="1"/>
       <c r="AI164" s="1"/>
       <c r="AJ164" s="3"/>
-      <c r="AK164" s="4"/>
+      <c r="AK164" s="5"/>
     </row>
     <row r="165" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
@@ -28864,7 +28870,7 @@
       <c r="AH165" s="1"/>
       <c r="AI165" s="1"/>
       <c r="AJ165" s="1"/>
-      <c r="AK165" s="4"/>
+      <c r="AK165" s="5"/>
     </row>
     <row r="166" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
@@ -28926,7 +28932,7 @@
       <c r="AH166" s="1"/>
       <c r="AI166" s="1"/>
       <c r="AJ166" s="3"/>
-      <c r="AK166" s="4"/>
+      <c r="AK166" s="5"/>
     </row>
     <row r="167" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
@@ -29000,7 +29006,7 @@
       <c r="AH167" s="1"/>
       <c r="AI167" s="1"/>
       <c r="AJ167" s="1"/>
-      <c r="AK167" s="4"/>
+      <c r="AK167" s="5"/>
     </row>
     <row r="168" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
@@ -29056,7 +29062,7 @@
       <c r="AH168" s="1"/>
       <c r="AI168" s="1"/>
       <c r="AJ168" s="2"/>
-      <c r="AK168" s="4"/>
+      <c r="AK168" s="5"/>
     </row>
     <row r="169" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
@@ -29118,7 +29124,7 @@
       <c r="AH169" s="1"/>
       <c r="AI169" s="1"/>
       <c r="AJ169" s="3"/>
-      <c r="AK169" s="4"/>
+      <c r="AK169" s="5"/>
     </row>
     <row r="170" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
@@ -29180,7 +29186,7 @@
       <c r="AH170" s="1"/>
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
-      <c r="AK170" s="4"/>
+      <c r="AK170" s="5"/>
     </row>
     <row r="171" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
@@ -29248,7 +29254,7 @@
       <c r="AH171" s="1"/>
       <c r="AI171" s="1"/>
       <c r="AJ171" s="3"/>
-      <c r="AK171" s="4"/>
+      <c r="AK171" s="5"/>
     </row>
     <row r="172" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
@@ -29310,7 +29316,7 @@
       <c r="AH172" s="1"/>
       <c r="AI172" s="1"/>
       <c r="AJ172" s="1"/>
-      <c r="AK172" s="4"/>
+      <c r="AK172" s="5"/>
     </row>
     <row r="173" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
@@ -29372,7 +29378,7 @@
       <c r="AH173" s="1"/>
       <c r="AI173" s="1"/>
       <c r="AJ173" s="3"/>
-      <c r="AK173" s="4"/>
+      <c r="AK173" s="5"/>
     </row>
     <row r="174" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
@@ -29434,7 +29440,7 @@
       <c r="AH174" s="1"/>
       <c r="AI174" s="1"/>
       <c r="AJ174" s="1"/>
-      <c r="AK174" s="4"/>
+      <c r="AK174" s="5"/>
     </row>
     <row r="175" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
@@ -29502,7 +29508,7 @@
       <c r="AH175" s="1"/>
       <c r="AI175" s="1"/>
       <c r="AJ175" s="2"/>
-      <c r="AK175" s="4"/>
+      <c r="AK175" s="5"/>
     </row>
     <row r="176" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
@@ -29564,7 +29570,7 @@
       <c r="AH176" s="1"/>
       <c r="AI176" s="1"/>
       <c r="AJ176" s="3"/>
-      <c r="AK176" s="4"/>
+      <c r="AK176" s="5"/>
     </row>
     <row r="177" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
@@ -29626,7 +29632,7 @@
       <c r="AH177" s="1"/>
       <c r="AI177" s="1"/>
       <c r="AJ177" s="1"/>
-      <c r="AK177" s="4"/>
+      <c r="AK177" s="5"/>
     </row>
     <row r="178" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
@@ -29688,7 +29694,7 @@
       <c r="AH178" s="1"/>
       <c r="AI178" s="1"/>
       <c r="AJ178" s="3"/>
-      <c r="AK178" s="4"/>
+      <c r="AK178" s="5"/>
     </row>
     <row r="179" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
@@ -29762,7 +29768,7 @@
       <c r="AH179" s="1"/>
       <c r="AI179" s="1"/>
       <c r="AJ179" s="1"/>
-      <c r="AK179" s="4"/>
+      <c r="AK179" s="5"/>
     </row>
     <row r="180" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>

</xml_diff>

<commit_message>
All classes are finished and excel file updated
</commit_message>
<xml_diff>
--- a/Satisfactory_calculator/item_list.xlsx
+++ b/Satisfactory_calculator/item_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjarki\source\repos\Satisfactory_calculator\Satisfactory_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4CFEAD-CA80-44D9-9E70-BA1B3C25050C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA3EDDF-A143-403A-9C5A-2846FF9D9C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2760" windowWidth="30405" windowHeight="14295" activeTab="3" xr2:uid="{CF63DFE2-E3F1-40A6-9DC4-F78A2094206C}"/>
+    <workbookView xWindow="5340" yWindow="2760" windowWidth="30405" windowHeight="14295" xr2:uid="{CF63DFE2-E3F1-40A6-9DC4-F78A2094206C}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_material" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8234" uniqueCount="1348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8234" uniqueCount="1346">
   <si>
     <t>Crafted In</t>
   </si>
@@ -4071,12 +4071,6 @@
   </si>
   <si>
     <t>Dissolved Silica</t>
-  </si>
-  <si>
-    <t>item_qty_1</t>
-  </si>
-  <si>
-    <t>item_qty_unit_1</t>
   </si>
 </sst>
 </file>
@@ -7070,7 +7064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841FB181-CBC0-4A34-86F6-94FA4ACCE032}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -7292,8 +7286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C4349C-A20E-4466-BDDA-F12F53635295}">
   <dimension ref="A1:V316"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244:XFD244"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7330,10 +7324,10 @@
         <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>1346</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>1347</v>
+        <v>119</v>
       </c>
       <c r="E1" t="s">
         <v>1328</v>
@@ -21778,8 +21772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F544B06-6065-4C8E-AAF6-1E1D3DDA6940}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B57" sqref="B56:B57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Overclock factor implemented in classes, but are calculated incorrectly at some places. Need to debug both of them
</commit_message>
<xml_diff>
--- a/Satisfactory_calculator/item_list.xlsx
+++ b/Satisfactory_calculator/item_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bjarki\source\repos\Satisfactory_calculator\Satisfactory_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA3EDDF-A143-403A-9C5A-2846FF9D9C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C039C09-F41E-4D51-B71F-486ADD3ADEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="2760" windowWidth="30405" windowHeight="14295" xr2:uid="{CF63DFE2-E3F1-40A6-9DC4-F78A2094206C}"/>
+    <workbookView xWindow="5340" yWindow="2760" windowWidth="30405" windowHeight="14295" activeTab="3" xr2:uid="{CF63DFE2-E3F1-40A6-9DC4-F78A2094206C}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_material" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8234" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8237" uniqueCount="1347">
   <si>
     <t>Crafted In</t>
   </si>
@@ -4071,6 +4071,9 @@
   </si>
   <si>
     <t>Dissolved Silica</t>
+  </si>
+  <si>
+    <t>node</t>
   </si>
 </sst>
 </file>
@@ -7062,10 +7065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841FB181-CBC0-4A34-86F6-94FA4ACCE032}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7077,7 +7080,7 @@
     <col min="5" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -7096,8 +7099,11 @@
       <c r="F1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7116,8 +7122,11 @@
       <c r="F2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -7136,8 +7145,11 @@
       <c r="F3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -7156,8 +7168,11 @@
       <c r="F4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -7176,8 +7191,11 @@
       <c r="F5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -7196,8 +7214,11 @@
       <c r="F6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -7216,8 +7237,11 @@
       <c r="F7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -7236,8 +7260,11 @@
       <c r="F8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -7256,8 +7283,11 @@
       <c r="F9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -7275,6 +7305,9 @@
       </c>
       <c r="F10" t="s">
         <v>138</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7286,7 +7319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C4349C-A20E-4466-BDDA-F12F53635295}">
   <dimension ref="A1:V316"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -21397,7 +21430,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21762,6 +21795,15 @@
       <c r="D14" t="s">
         <v>83</v>
       </c>
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21772,8 +21814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F544B06-6065-4C8E-AAF6-1E1D3DDA6940}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21914,7 +21956,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>